<commit_message>
Add duplicate detection for contract note imports
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/ABB India Ltd.xlsx
+++ b/dumps/Stocks/ABB India Ltd.xlsx
@@ -19,10 +19,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$₹]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -239,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -385,6 +386,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +715,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP993"/>
+  <dimension ref="A1:AP994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
@@ -1062,8 +1064,8 @@
       <c r="AP4" s="1" t="n"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="61">
-      <c r="A5" s="72" t="n">
-        <v>46049</v>
+      <c r="A5" s="73" t="n">
+        <v>46063</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1072,33 +1074,33 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>4676</v>
+        <v>5777.1467</v>
       </c>
       <c r="F5" t="n">
-        <v>4709.13</v>
+        <v>17331.44</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252611730667</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>4.68</v>
+        <v>17.41</v>
       </c>
       <c r="I5" t="n">
-        <v>28.45</v>
+        <v>103.65</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="61">
       <c r="A6" s="72" t="n">
-        <v>46043</v>
+        <v>46049</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1111,13 +1113,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>4691.5</v>
+        <v>4676</v>
       </c>
       <c r="F6" t="n">
-        <v>9449.110000000001</v>
+        <v>4709.13</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1125,15 +1127,15 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>9.23</v>
+        <v>4.68</v>
       </c>
       <c r="I6" t="n">
-        <v>56.88</v>
+        <v>28.45</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="61">
       <c r="A7" s="72" t="n">
-        <v>46038</v>
+        <v>46043</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1146,13 +1148,13 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>4954.5</v>
+        <v>4691.5</v>
       </c>
       <c r="F7" t="n">
-        <v>4989.59</v>
+        <v>9449.110000000001</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1160,15 +1162,15 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>4.95</v>
+        <v>9.23</v>
       </c>
       <c r="I7" t="n">
-        <v>30.14</v>
+        <v>56.88</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="61">
       <c r="A8" s="72" t="n">
-        <v>46034</v>
+        <v>46038</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1184,10 +1186,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>5009</v>
+        <v>4954.5</v>
       </c>
       <c r="F8" t="n">
-        <v>5044.49</v>
+        <v>4989.59</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1195,15 +1197,15 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>5.02</v>
+        <v>4.95</v>
       </c>
       <c r="I8" t="n">
-        <v>30.47</v>
+        <v>30.14</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="61">
       <c r="A9" s="72" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1219,10 +1221,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>5157</v>
+        <v>5009</v>
       </c>
       <c r="F9" t="n">
-        <v>5193.53</v>
+        <v>5044.49</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1230,15 +1232,15 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>5.14</v>
+        <v>5.02</v>
       </c>
       <c r="I9" t="n">
-        <v>31.39</v>
+        <v>30.47</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="61">
       <c r="A10" s="72" t="n">
-        <v>46020</v>
+        <v>46030</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1254,10 +1256,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>5180.5</v>
+        <v>5157</v>
       </c>
       <c r="F10" t="n">
-        <v>5217.26</v>
+        <v>5193.53</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1265,15 +1267,15 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>5.2</v>
+        <v>5.14</v>
       </c>
       <c r="I10" t="n">
-        <v>31.56</v>
+        <v>31.39</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="61">
       <c r="A11" s="72" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1289,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>5232</v>
+        <v>5180.5</v>
       </c>
       <c r="F11" t="n">
-        <v>5269.08</v>
+        <v>5217.26</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1300,15 +1302,15 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>5.25</v>
+        <v>5.2</v>
       </c>
       <c r="I11" t="n">
-        <v>31.83</v>
+        <v>31.56</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="61">
       <c r="A12" s="72" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1324,10 +1326,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>5244.5</v>
+        <v>5232</v>
       </c>
       <c r="F12" t="n">
-        <v>5281.65</v>
+        <v>5269.08</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1335,15 +1337,15 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>5.21</v>
+        <v>5.25</v>
       </c>
       <c r="I12" t="n">
-        <v>31.94</v>
+        <v>31.83</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="61">
       <c r="A13" s="72" t="n">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1359,10 +1361,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>5187.5</v>
+        <v>5244.5</v>
       </c>
       <c r="F13" t="n">
-        <v>5224.24</v>
+        <v>5281.65</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1370,19 +1372,19 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>5.17</v>
+        <v>5.21</v>
       </c>
       <c r="I13" t="n">
-        <v>31.57</v>
+        <v>31.94</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="61">
       <c r="A14" s="72" t="n">
-        <v>46009</v>
+        <v>46014</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1394,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>5116</v>
+        <v>5187.5</v>
       </c>
       <c r="F14" t="n">
-        <v>5152.32</v>
+        <v>5224.24</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1405,15 +1407,15 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>5.13</v>
+        <v>5.17</v>
       </c>
       <c r="I14" t="n">
-        <v>31.19</v>
+        <v>31.57</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="61">
       <c r="A15" s="72" t="n">
-        <v>46007</v>
+        <v>46009</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1429,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>5268.75</v>
+        <v>5116</v>
       </c>
       <c r="F15" t="n">
-        <v>5306.15</v>
+        <v>5152.32</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1440,15 +1442,15 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>5.26</v>
+        <v>5.13</v>
       </c>
       <c r="I15" t="n">
-        <v>32.14</v>
+        <v>31.19</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="61">
       <c r="A16" s="72" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1464,10 +1466,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>5211.65</v>
+        <v>5268.75</v>
       </c>
       <c r="F16" t="n">
-        <v>5248.71</v>
+        <v>5306.15</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1475,19 +1477,19 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>5.24</v>
+        <v>5.26</v>
       </c>
       <c r="I16" t="n">
-        <v>31.82</v>
+        <v>32.14</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="61">
       <c r="A17" s="72" t="n">
-        <v>45971</v>
+        <v>46006</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1496,13 +1498,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>4987</v>
+        <v>5211.65</v>
       </c>
       <c r="F17" t="n">
-        <v>10044.63</v>
+        <v>5248.71</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1510,15 +1512,15 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>9.92</v>
+        <v>5.24</v>
       </c>
       <c r="I17" t="n">
-        <v>60.71</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="61">
       <c r="A18" s="72" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1534,10 +1536,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>5032.5</v>
+        <v>4987</v>
       </c>
       <c r="F18" t="n">
-        <v>10136.32</v>
+        <v>10044.63</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1545,19 +1547,19 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>10.05</v>
+        <v>9.92</v>
       </c>
       <c r="I18" t="n">
-        <v>61.27</v>
+        <v>60.71</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="61">
       <c r="A19" s="72" t="n">
-        <v>45957</v>
+        <v>45968</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1569,10 +1571,10 @@
         <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>5210.75</v>
+        <v>5032.5</v>
       </c>
       <c r="F19" t="n">
-        <v>10495.49</v>
+        <v>10136.32</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1580,19 +1582,19 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>10.46</v>
+        <v>10.05</v>
       </c>
       <c r="I19" t="n">
-        <v>63.53</v>
+        <v>61.27</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="61">
       <c r="A20" s="72" t="n">
-        <v>45954</v>
+        <v>45957</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1604,10 +1606,10 @@
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>5196.5</v>
+        <v>5210.75</v>
       </c>
       <c r="F20" t="n">
-        <v>10466.7</v>
+        <v>10495.49</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1615,15 +1617,15 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>10.41</v>
+        <v>10.46</v>
       </c>
       <c r="I20" t="n">
-        <v>63.29</v>
+        <v>63.53</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="61">
       <c r="A21" s="72" t="n">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1639,10 +1641,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>5240</v>
+        <v>5196.5</v>
       </c>
       <c r="F21" t="n">
-        <v>10554.25</v>
+        <v>10466.7</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1650,15 +1652,15 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>10.44</v>
+        <v>10.41</v>
       </c>
       <c r="I21" t="n">
-        <v>63.81</v>
+        <v>63.29</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="61">
       <c r="A22" s="72" t="n">
-        <v>45950</v>
+        <v>45953</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1674,10 +1676,10 @@
         <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>5239</v>
+        <v>5240</v>
       </c>
       <c r="F22" t="n">
-        <v>10552.28</v>
+        <v>10554.25</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1685,7 +1687,7 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>10.47</v>
+        <v>10.44</v>
       </c>
       <c r="I22" t="n">
         <v>63.81</v>
@@ -1693,11 +1695,11 @@
     </row>
     <row r="23" ht="15.75" customHeight="1" s="61">
       <c r="A23" s="72" t="n">
-        <v>45947</v>
+        <v>45950</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1709,10 +1711,10 @@
         <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>5195.3</v>
+        <v>5239</v>
       </c>
       <c r="F23" t="n">
-        <v>10464.36</v>
+        <v>10552.28</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1720,19 +1722,19 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>10.42</v>
+        <v>10.47</v>
       </c>
       <c r="I23" t="n">
-        <v>63.34</v>
+        <v>63.81</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="61">
       <c r="A24" s="72" t="n">
-        <v>45924</v>
+        <v>45947</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1741,13 +1743,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>5316.6</v>
+        <v>5195.3</v>
       </c>
       <c r="F24" t="n">
-        <v>5354.25</v>
+        <v>10464.36</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1755,10 +1757,10 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>5.3</v>
+        <v>10.42</v>
       </c>
       <c r="I24" t="n">
-        <v>32.35</v>
+        <v>63.34</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="61">
@@ -1779,10 +1781,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>5316.7</v>
+        <v>5316.6</v>
       </c>
       <c r="F25" t="n">
-        <v>5354.39</v>
+        <v>5354.25</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1793,16 +1795,16 @@
         <v>5.3</v>
       </c>
       <c r="I25" t="n">
-        <v>32.39</v>
+        <v>32.35</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="61">
       <c r="A26" s="72" t="n">
-        <v>45903</v>
+        <v>45924</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1811,13 +1813,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>5192.65</v>
+        <v>5316.7</v>
       </c>
       <c r="F26" t="n">
-        <v>10459.02</v>
+        <v>5354.39</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1825,120 +1827,54 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>10.41</v>
+        <v>5.3</v>
       </c>
       <c r="I26" t="n">
-        <v>63.31</v>
+        <v>32.39</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="61">
-      <c r="A27" s="25" t="n">
-        <v>45877</v>
-      </c>
-      <c r="B27" s="26" t="inlineStr">
+      <c r="A27" s="72" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
-          <t>DIV</t>
+          <t>BSE</t>
         </is>
       </c>
-      <c r="C27" s="26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D27" s="27" t="n">
-        <v>15</v>
-      </c>
-      <c r="E27" s="28" t="n">
-        <v>9.77</v>
-      </c>
-      <c r="F27" s="28" t="n">
-        <v>146.55</v>
-      </c>
-      <c r="G27" s="26" t="inlineStr">
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5192.65</v>
+      </c>
+      <c r="F27" t="n">
+        <v>10459.02</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
-          <t>Interim-Dividend of Rs.9.7700/- per share on Ex-Date: 08-AUG-2025</t>
+          <t>~</t>
         </is>
       </c>
-      <c r="H27" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="29">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K27" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
-        <v/>
-      </c>
-      <c r="L27" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
-        <v/>
-      </c>
-      <c r="M27" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
-        <v/>
-      </c>
-      <c r="N27" s="32">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
-        <v/>
-      </c>
-      <c r="O27" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
-        <v/>
-      </c>
-      <c r="P27" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
-        <v/>
-      </c>
-      <c r="Q27" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
-        <v/>
-      </c>
-      <c r="R27" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
-        <v/>
-      </c>
-      <c r="S27" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
-        <v/>
-      </c>
-      <c r="T27" s="34">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
-        <v/>
-      </c>
-      <c r="U27" s="34">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
-        <v/>
-      </c>
-      <c r="V27" s="34">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
-        <v/>
-      </c>
-      <c r="W27" s="34" t="n"/>
-      <c r="X27" s="34" t="n"/>
-      <c r="Y27" s="33">
-        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
-        <v/>
-      </c>
-      <c r="Z27" s="34" t="n"/>
-      <c r="AA27" s="34" t="n"/>
-      <c r="AB27" s="35" t="n"/>
-      <c r="AC27" s="31">
-        <f>IF(B13="DIV", F13,"")</f>
-        <v/>
-      </c>
-      <c r="AD27" s="36" t="n"/>
+      <c r="H27" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="I27" t="n">
+        <v>63.31</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="61">
       <c r="A28" s="25" t="n">
-        <v>45820</v>
+        <v>45877</v>
       </c>
       <c r="B28" s="26" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>DIV</t>
         </is>
       </c>
       <c r="C28" s="26" t="inlineStr">
@@ -1947,95 +1883,95 @@
         </is>
       </c>
       <c r="D28" s="27" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E28" s="28" t="n">
-        <v>6102.91</v>
+        <v>9.77</v>
       </c>
       <c r="F28" s="28" t="n">
-        <v>12205.83</v>
+        <v>146.55</v>
       </c>
       <c r="G28" s="26" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>Interim-Dividend of Rs.9.7700/- per share on Ex-Date: 08-AUG-2025</t>
         </is>
       </c>
       <c r="H28" s="27" t="n">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="27" t="n">
-        <v>73.73</v>
+        <v>0</v>
       </c>
       <c r="J28" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K28" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="L28" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="M28" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
         <v/>
       </c>
       <c r="N28" s="32">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
         <v/>
       </c>
       <c r="O28" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="P28" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="Q28" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
         <v/>
       </c>
       <c r="R28" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="S28" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="T28" s="34">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="U28" s="34">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
         <v/>
       </c>
       <c r="V28" s="34">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="W28" s="34" t="n"/>
       <c r="X28" s="34" t="n"/>
       <c r="Y28" s="33">
-        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="Z28" s="34" t="n"/>
       <c r="AA28" s="34" t="n"/>
       <c r="AB28" s="35" t="n"/>
       <c r="AC28" s="31">
-        <f>IF(B14="DIV", F14,"")</f>
+        <f>IF(B13="DIV", F13,"")</f>
         <v/>
       </c>
       <c r="AD28" s="36" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="61">
       <c r="A29" s="25" t="n">
-        <v>45813</v>
+        <v>45820</v>
       </c>
       <c r="B29" s="26" t="inlineStr">
         <is>
@@ -2048,13 +1984,13 @@
         </is>
       </c>
       <c r="D29" s="27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="28" t="n">
-        <v>6088.55</v>
+        <v>6102.91</v>
       </c>
       <c r="F29" s="28" t="n">
-        <v>6088.55</v>
+        <v>12205.83</v>
       </c>
       <c r="G29" s="26" t="inlineStr">
         <is>
@@ -2062,81 +1998,81 @@
         </is>
       </c>
       <c r="H29" s="27" t="n">
-        <v>5.69</v>
+        <v>12.1</v>
       </c>
       <c r="I29" s="27" t="n">
-        <v>36.86</v>
+        <v>73.73</v>
       </c>
       <c r="J29" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K29" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="L29" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="M29" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
         <v/>
       </c>
       <c r="N29" s="32">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
         <v/>
       </c>
       <c r="O29" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="P29" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="Q29" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
         <v/>
       </c>
       <c r="R29" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="S29" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="T29" s="34">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="U29" s="34">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
         <v/>
       </c>
       <c r="V29" s="34">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="W29" s="34" t="n"/>
       <c r="X29" s="34" t="n"/>
       <c r="Y29" s="33">
-        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="Z29" s="34" t="n"/>
       <c r="AA29" s="34" t="n"/>
       <c r="AB29" s="35" t="n"/>
       <c r="AC29" s="31">
-        <f>IF(B15="DIV", F15,"")</f>
+        <f>IF(B14="DIV", F14,"")</f>
         <v/>
       </c>
       <c r="AD29" s="36" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="61">
       <c r="A30" s="25" t="n">
-        <v>45811</v>
+        <v>45813</v>
       </c>
       <c r="B30" s="26" t="inlineStr">
         <is>
@@ -2149,13 +2085,13 @@
         </is>
       </c>
       <c r="D30" s="27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="28" t="n">
-        <v>6105.48</v>
+        <v>6088.55</v>
       </c>
       <c r="F30" s="28" t="n">
-        <v>12210.97</v>
+        <v>6088.55</v>
       </c>
       <c r="G30" s="26" t="inlineStr">
         <is>
@@ -2163,85 +2099,85 @@
         </is>
       </c>
       <c r="H30" s="27" t="n">
-        <v>12.13</v>
+        <v>5.69</v>
       </c>
       <c r="I30" s="27" t="n">
-        <v>73.84</v>
+        <v>36.86</v>
       </c>
       <c r="J30" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K30" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="L30" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="M30" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
         <v/>
       </c>
       <c r="N30" s="32">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
         <v/>
       </c>
       <c r="O30" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="P30" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="Q30" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
         <v/>
       </c>
       <c r="R30" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="S30" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="T30" s="34">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="U30" s="34">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
         <v/>
       </c>
       <c r="V30" s="34">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="W30" s="34" t="n"/>
       <c r="X30" s="34" t="n"/>
       <c r="Y30" s="33">
-        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="Z30" s="34" t="n"/>
       <c r="AA30" s="34" t="n"/>
       <c r="AB30" s="35" t="n"/>
       <c r="AC30" s="31">
-        <f>IF(B16="DIV", F16,"")</f>
+        <f>IF(B15="DIV", F15,"")</f>
         <v/>
       </c>
       <c r="AD30" s="36" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="61">
       <c r="A31" s="25" t="n">
-        <v>45779</v>
+        <v>45811</v>
       </c>
       <c r="B31" s="26" t="inlineStr">
         <is>
-          <t>DIV</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C31" s="26" t="inlineStr">
@@ -2250,195 +2186,196 @@
         </is>
       </c>
       <c r="D31" s="27" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E31" s="28" t="n">
-        <v>33.5</v>
+        <v>6105.48</v>
       </c>
       <c r="F31" s="28" t="n">
-        <v>335</v>
+        <v>12210.97</v>
       </c>
       <c r="G31" s="26" t="inlineStr">
         <is>
-          <t>Final-Dividend of Rs.33.5000/- per share on Ex-Date: 02-MAY-2025</t>
+          <t>~</t>
         </is>
       </c>
       <c r="H31" s="27" t="n">
-        <v>0</v>
+        <v>12.13</v>
       </c>
       <c r="I31" s="27" t="n">
-        <v>0</v>
+        <v>73.84</v>
       </c>
       <c r="J31" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K31" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="L31" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="M31" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
         <v/>
       </c>
       <c r="N31" s="32">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
         <v/>
       </c>
       <c r="O31" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="P31" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="Q31" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
         <v/>
       </c>
       <c r="R31" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="S31" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="T31" s="34">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="U31" s="34">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
         <v/>
       </c>
       <c r="V31" s="34">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="W31" s="34" t="n"/>
       <c r="X31" s="34" t="n"/>
       <c r="Y31" s="33">
-        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="Z31" s="34" t="n"/>
       <c r="AA31" s="34" t="n"/>
       <c r="AB31" s="35" t="n"/>
       <c r="AC31" s="31">
-        <f>IF(B17="DIV", F17,"")</f>
+        <f>IF(B16="DIV", F16,"")</f>
         <v/>
       </c>
       <c r="AD31" s="36" t="n"/>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="61">
-      <c r="A32" s="37" t="n">
-        <v>45734</v>
-      </c>
-      <c r="B32" s="38" t="inlineStr">
+      <c r="A32" s="25" t="n">
+        <v>45779</v>
+      </c>
+      <c r="B32" s="26" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>DIV</t>
         </is>
       </c>
-      <c r="C32" s="38" t="inlineStr">
+      <c r="C32" s="26" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D32" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="40" t="n">
-        <v>5407.11</v>
-      </c>
-      <c r="F32" s="40">
-        <f>D18*E18</f>
-        <v/>
-      </c>
-      <c r="G32" s="38" t="inlineStr">
+      <c r="D32" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E32" s="28" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="F32" s="28" t="n">
+        <v>335</v>
+      </c>
+      <c r="G32" s="26" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>Final-Dividend of Rs.33.5000/- per share on Ex-Date: 02-MAY-2025</t>
         </is>
       </c>
-      <c r="H32" s="39" t="n"/>
-      <c r="I32" s="39" t="n">
-        <v>38.11</v>
+      <c r="H32" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="27" t="n">
+        <v>0</v>
       </c>
       <c r="J32" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K32" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="L32" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="M32" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
         <v/>
       </c>
       <c r="N32" s="32">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
         <v/>
       </c>
       <c r="O32" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="P32" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="Q32" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
         <v/>
       </c>
       <c r="R32" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="S32" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="T32" s="34">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="U32" s="34">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
         <v/>
       </c>
       <c r="V32" s="34">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="W32" s="34" t="n"/>
       <c r="X32" s="34" t="n"/>
       <c r="Y32" s="33">
-        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="Z32" s="34" t="n"/>
       <c r="AA32" s="34" t="n"/>
       <c r="AB32" s="35" t="n"/>
       <c r="AC32" s="31">
-        <f>IF(B18="DIV", F18,"")</f>
+        <f>IF(B17="DIV", F17,"")</f>
         <v/>
       </c>
       <c r="AD32" s="36" t="n"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="61">
       <c r="A33" s="37" t="n">
-        <v>45722</v>
+        <v>45734</v>
       </c>
       <c r="B33" s="38" t="inlineStr">
         <is>
@@ -2454,92 +2391,91 @@
         <v>1</v>
       </c>
       <c r="E33" s="40" t="n">
-        <v>5413.19</v>
-      </c>
-      <c r="F33" s="40" t="n">
-        <v>5413.19</v>
+        <v>5407.11</v>
+      </c>
+      <c r="F33" s="40">
+        <f>D18*E18</f>
+        <v/>
       </c>
       <c r="G33" s="38" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H33" s="39" t="n">
-        <v>5.4</v>
-      </c>
+      <c r="H33" s="39" t="n"/>
       <c r="I33" s="39" t="n">
-        <v>32.74</v>
+        <v>38.11</v>
       </c>
       <c r="J33" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K33" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="L33" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="M33" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
         <v/>
       </c>
       <c r="N33" s="32">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
         <v/>
       </c>
       <c r="O33" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="P33" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="Q33" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
         <v/>
       </c>
       <c r="R33" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="S33" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="T33" s="34">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="U33" s="34">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
         <v/>
       </c>
       <c r="V33" s="34">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="W33" s="34" t="n"/>
       <c r="X33" s="34" t="n"/>
       <c r="Y33" s="33">
-        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="Z33" s="34" t="n"/>
       <c r="AA33" s="34" t="n"/>
       <c r="AB33" s="35" t="n"/>
       <c r="AC33" s="31">
-        <f>IF(B19="DIV", F19,"")</f>
+        <f>IF(B18="DIV", F18,"")</f>
         <v/>
       </c>
       <c r="AD33" s="36" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="61">
       <c r="A34" s="37" t="n">
-        <v>45716</v>
+        <v>45722</v>
       </c>
       <c r="B34" s="38" t="inlineStr">
         <is>
@@ -2555,10 +2491,10 @@
         <v>1</v>
       </c>
       <c r="E34" s="40" t="n">
-        <v>5062.5</v>
+        <v>5413.19</v>
       </c>
       <c r="F34" s="40" t="n">
-        <v>5062.5</v>
+        <v>5413.19</v>
       </c>
       <c r="G34" s="38" t="inlineStr">
         <is>
@@ -2566,81 +2502,81 @@
         </is>
       </c>
       <c r="H34" s="39" t="n">
-        <v>5.02</v>
+        <v>5.4</v>
       </c>
       <c r="I34" s="39" t="n">
-        <v>30.58</v>
+        <v>32.74</v>
       </c>
       <c r="J34" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K34" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="L34" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="M34" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
         <v/>
       </c>
       <c r="N34" s="32">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
         <v/>
       </c>
       <c r="O34" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="P34" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="Q34" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
         <v/>
       </c>
       <c r="R34" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="S34" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="T34" s="34">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="U34" s="34">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
         <v/>
       </c>
       <c r="V34" s="34">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="W34" s="34" t="n"/>
       <c r="X34" s="34" t="n"/>
       <c r="Y34" s="33">
-        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="Z34" s="34" t="n"/>
       <c r="AA34" s="34" t="n"/>
       <c r="AB34" s="35" t="n"/>
       <c r="AC34" s="31">
-        <f>IF(B20="DIV", F20,"")</f>
+        <f>IF(B19="DIV", F19,"")</f>
         <v/>
       </c>
       <c r="AD34" s="36" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="61">
       <c r="A35" s="37" t="n">
-        <v>45712</v>
+        <v>45716</v>
       </c>
       <c r="B35" s="38" t="inlineStr">
         <is>
@@ -2656,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="E35" s="40" t="n">
-        <v>5353.01</v>
+        <v>5062.5</v>
       </c>
       <c r="F35" s="40" t="n">
-        <v>5353.01</v>
+        <v>5062.5</v>
       </c>
       <c r="G35" s="38" t="inlineStr">
         <is>
@@ -2667,81 +2603,81 @@
         </is>
       </c>
       <c r="H35" s="39" t="n">
-        <v>5.31</v>
+        <v>5.02</v>
       </c>
       <c r="I35" s="39" t="n">
-        <v>32.35</v>
+        <v>30.58</v>
       </c>
       <c r="J35" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K35" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="L35" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="M35" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
         <v/>
       </c>
       <c r="N35" s="32">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
         <v/>
       </c>
       <c r="O35" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="P35" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="Q35" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
         <v/>
       </c>
       <c r="R35" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="S35" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="T35" s="34">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="U35" s="34">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
         <v/>
       </c>
       <c r="V35" s="34">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="W35" s="34" t="n"/>
       <c r="X35" s="34" t="n"/>
       <c r="Y35" s="33">
-        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="Z35" s="34" t="n"/>
       <c r="AA35" s="34" t="n"/>
       <c r="AB35" s="35" t="n"/>
       <c r="AC35" s="31">
-        <f>IF(B21="DIV", F21,"")</f>
+        <f>IF(B20="DIV", F20,"")</f>
         <v/>
       </c>
       <c r="AD35" s="36" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="61">
       <c r="A36" s="37" t="n">
-        <v>45708</v>
+        <v>45712</v>
       </c>
       <c r="B36" s="38" t="inlineStr">
         <is>
@@ -2757,10 +2693,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="40" t="n">
-        <v>5226.61</v>
+        <v>5353.01</v>
       </c>
       <c r="F36" s="40" t="n">
-        <v>5226.61</v>
+        <v>5353.01</v>
       </c>
       <c r="G36" s="38" t="inlineStr">
         <is>
@@ -2768,74 +2704,74 @@
         </is>
       </c>
       <c r="H36" s="39" t="n">
-        <v>5.17</v>
+        <v>5.31</v>
       </c>
       <c r="I36" s="39" t="n">
-        <v>31.49</v>
+        <v>32.35</v>
       </c>
       <c r="J36" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K36" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="L36" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="M36" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
         <v/>
       </c>
       <c r="N36" s="32">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
         <v/>
       </c>
       <c r="O36" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="P36" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="Q36" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
         <v/>
       </c>
       <c r="R36" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="S36" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="T36" s="34">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="U36" s="34">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
         <v/>
       </c>
       <c r="V36" s="34">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="W36" s="34" t="n"/>
       <c r="X36" s="34" t="n"/>
       <c r="Y36" s="33">
-        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="Z36" s="34" t="n"/>
       <c r="AA36" s="34" t="n"/>
       <c r="AB36" s="35" t="n"/>
       <c r="AC36" s="31">
-        <f>IF(B22="DIV", F22,"")</f>
+        <f>IF(B21="DIV", F21,"")</f>
         <v/>
       </c>
       <c r="AD36" s="36" t="n"/>
@@ -2858,10 +2794,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="40" t="n">
-        <v>5226.67</v>
+        <v>5226.61</v>
       </c>
       <c r="F37" s="40" t="n">
-        <v>5226.67</v>
+        <v>5226.61</v>
       </c>
       <c r="G37" s="38" t="inlineStr">
         <is>
@@ -2872,78 +2808,78 @@
         <v>5.17</v>
       </c>
       <c r="I37" s="39" t="n">
-        <v>31.5</v>
+        <v>31.49</v>
       </c>
       <c r="J37" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K37" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="L37" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="M37" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
         <v/>
       </c>
       <c r="N37" s="32">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
         <v/>
       </c>
       <c r="O37" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="P37" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="Q37" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
         <v/>
       </c>
       <c r="R37" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="S37" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="T37" s="34">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="U37" s="34">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
         <v/>
       </c>
       <c r="V37" s="34">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="W37" s="34" t="n"/>
       <c r="X37" s="34" t="n"/>
       <c r="Y37" s="33">
-        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="Z37" s="34" t="n"/>
       <c r="AA37" s="34" t="n"/>
       <c r="AB37" s="35" t="n"/>
       <c r="AC37" s="31">
-        <f>IF(B23="DIV", F23,"")</f>
+        <f>IF(B22="DIV", F22,"")</f>
         <v/>
       </c>
       <c r="AD37" s="36" t="n"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="61">
       <c r="A38" s="37" t="n">
-        <v>45705</v>
+        <v>45708</v>
       </c>
       <c r="B38" s="38" t="inlineStr">
         <is>
@@ -2956,13 +2892,13 @@
         </is>
       </c>
       <c r="D38" s="39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="40" t="n">
-        <v>5300.31</v>
+        <v>5226.67</v>
       </c>
       <c r="F38" s="40" t="n">
-        <v>10600.61</v>
+        <v>5226.67</v>
       </c>
       <c r="G38" s="38" t="inlineStr">
         <is>
@@ -2970,81 +2906,81 @@
         </is>
       </c>
       <c r="H38" s="39" t="n">
-        <v>10.52</v>
+        <v>5.17</v>
       </c>
       <c r="I38" s="39" t="n">
-        <v>64.09</v>
+        <v>31.5</v>
       </c>
       <c r="J38" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K38" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="L38" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="M38" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
         <v/>
       </c>
       <c r="N38" s="32">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
         <v/>
       </c>
       <c r="O38" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="P38" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="Q38" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
         <v/>
       </c>
       <c r="R38" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="S38" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="T38" s="34">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="U38" s="34">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
         <v/>
       </c>
       <c r="V38" s="34">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="W38" s="34" t="n"/>
       <c r="X38" s="34" t="n"/>
       <c r="Y38" s="33">
-        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="Z38" s="34" t="n"/>
       <c r="AA38" s="34" t="n"/>
       <c r="AB38" s="35" t="n"/>
       <c r="AC38" s="31">
-        <f>IF(B24="DIV", F24,"")</f>
+        <f>IF(B23="DIV", F23,"")</f>
         <v/>
       </c>
       <c r="AD38" s="36" t="n"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="61">
       <c r="A39" s="37" t="n">
-        <v>45699</v>
+        <v>45705</v>
       </c>
       <c r="B39" s="38" t="inlineStr">
         <is>
@@ -3057,13 +2993,13 @@
         </is>
       </c>
       <c r="D39" s="39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="40" t="n">
-        <v>5524.45</v>
+        <v>5300.31</v>
       </c>
       <c r="F39" s="40" t="n">
-        <v>5524.45</v>
+        <v>10600.61</v>
       </c>
       <c r="G39" s="38" t="inlineStr">
         <is>
@@ -3071,74 +3007,74 @@
         </is>
       </c>
       <c r="H39" s="39" t="n">
-        <v>5.49</v>
+        <v>10.52</v>
       </c>
       <c r="I39" s="39" t="n">
-        <v>33.41</v>
+        <v>64.09</v>
       </c>
       <c r="J39" s="29">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K39" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="L39" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="M39" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
         <v/>
       </c>
       <c r="N39" s="32">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
         <v/>
       </c>
       <c r="O39" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="P39" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="Q39" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
         <v/>
       </c>
       <c r="R39" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
         <v/>
       </c>
       <c r="S39" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="T39" s="34">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="U39" s="34">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
         <v/>
       </c>
       <c r="V39" s="34">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
         <v/>
       </c>
       <c r="W39" s="34" t="n"/>
       <c r="X39" s="34" t="n"/>
       <c r="Y39" s="33">
-        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="Z39" s="34" t="n"/>
       <c r="AA39" s="34" t="n"/>
       <c r="AB39" s="35" t="n"/>
       <c r="AC39" s="31">
-        <f>IF(B25="DIV", F25,"")</f>
+        <f>IF(B24="DIV", F24,"")</f>
         <v/>
       </c>
       <c r="AD39" s="36" t="n"/>
@@ -3182,83 +3118,168 @@
         <v/>
       </c>
       <c r="K40" s="30">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), L26/SUM(F26:I26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
         <v/>
       </c>
       <c r="L40" s="31">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
         <v/>
       </c>
       <c r="M40" s="31">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), ((E26*D26)+L26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
         <v/>
       </c>
       <c r="N40" s="32">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), D26, "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
         <v/>
       </c>
       <c r="O40" s="30">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), P26/SUM(F26:I26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
         <v/>
       </c>
       <c r="P40" s="31">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
         <v/>
       </c>
       <c r="Q40" s="31">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), ((E26*D26)+P26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
         <v/>
       </c>
       <c r="R40" s="31">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), D26, "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
         <v/>
       </c>
       <c r="S40" s="33">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), T26/SUM(F26:I26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
         <v/>
       </c>
       <c r="T40" s="34">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
         <v/>
       </c>
       <c r="U40" s="34">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), ((E26*D26)+T26), "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
         <v/>
       </c>
       <c r="V40" s="34">
-        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), D26, "")</f>
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
         <v/>
       </c>
       <c r="W40" s="34" t="n"/>
       <c r="X40" s="34" t="n"/>
       <c r="Y40" s="33">
-        <f>IF(AND( C26="Buy", W26&lt;&gt;"", AA26&lt;&gt;"", B26&lt;&gt;"DIV"), Z26/SUM(F26:I26), "")</f>
+        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
         <v/>
       </c>
       <c r="Z40" s="34" t="n"/>
       <c r="AA40" s="34" t="n"/>
       <c r="AB40" s="35" t="n"/>
       <c r="AC40" s="31">
+        <f>IF(B25="DIV", F25,"")</f>
+        <v/>
+      </c>
+      <c r="AD40" s="36" t="n"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" s="61">
+      <c r="A41" s="37" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B41" s="38" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C41" s="38" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D41" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="40" t="n">
+        <v>5524.45</v>
+      </c>
+      <c r="F41" s="40" t="n">
+        <v>5524.45</v>
+      </c>
+      <c r="G41" s="38" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H41" s="39" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="I41" s="39" t="n">
+        <v>33.41</v>
+      </c>
+      <c r="J41" s="29">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K41" s="30">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), L26/SUM(F26:I26), "")</f>
+        <v/>
+      </c>
+      <c r="L41" s="31">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <v/>
+      </c>
+      <c r="M41" s="31">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), ((E26*D26)+L26), "")</f>
+        <v/>
+      </c>
+      <c r="N41" s="32">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV"), D26, "")</f>
+        <v/>
+      </c>
+      <c r="O41" s="30">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), P26/SUM(F26:I26), "")</f>
+        <v/>
+      </c>
+      <c r="P41" s="31">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <v/>
+      </c>
+      <c r="Q41" s="31">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), ((E26*D26)+P26), "")</f>
+        <v/>
+      </c>
+      <c r="R41" s="31">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &lt; 365), D26, "")</f>
+        <v/>
+      </c>
+      <c r="S41" s="33">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), T26/SUM(F26:I26), "")</f>
+        <v/>
+      </c>
+      <c r="T41" s="34">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), (1-Index!$F$2*2)*((J26*D26)-(E26*D26)), "")</f>
+        <v/>
+      </c>
+      <c r="U41" s="34">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), ((E26*D26)+T26), "")</f>
+        <v/>
+      </c>
+      <c r="V41" s="34">
+        <f>IF(AND( C26="Buy", ISBLANK(W26), B26&lt;&gt;"DIV", NOW()-A26 &gt; 365), D26, "")</f>
+        <v/>
+      </c>
+      <c r="W41" s="34" t="n"/>
+      <c r="X41" s="34" t="n"/>
+      <c r="Y41" s="33">
+        <f>IF(AND( C26="Buy", W26&lt;&gt;"", AA26&lt;&gt;"", B26&lt;&gt;"DIV"), Z26/SUM(F26:I26), "")</f>
+        <v/>
+      </c>
+      <c r="Z41" s="34" t="n"/>
+      <c r="AA41" s="34" t="n"/>
+      <c r="AB41" s="35" t="n"/>
+      <c r="AC41" s="31">
         <f>IF(B26="DIV", F26,"")</f>
         <v/>
       </c>
-      <c r="AD40" s="36" t="n"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1" s="61">
-      <c r="E41" s="41" t="n"/>
-      <c r="F41" s="41" t="n"/>
-      <c r="G41" s="42" t="n"/>
-      <c r="J41" s="41" t="n"/>
-      <c r="K41" s="41" t="n"/>
-      <c r="L41" s="41" t="n"/>
-      <c r="M41" s="1" t="n"/>
-      <c r="W41" s="41" t="n"/>
-      <c r="X41" s="41" t="n"/>
-      <c r="Y41" s="41" t="n"/>
-      <c r="Z41" s="41" t="n"/>
-      <c r="AA41" s="41" t="n"/>
-      <c r="AB41" s="41" t="n"/>
-      <c r="AC41" s="41" t="n"/>
+      <c r="AD41" s="36" t="n"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="61">
       <c r="E42" s="41" t="n"/>
@@ -18227,6 +18248,7 @@
       <c r="J977" s="41" t="n"/>
       <c r="K977" s="41" t="n"/>
       <c r="L977" s="41" t="n"/>
+      <c r="M977" s="1" t="n"/>
       <c r="W977" s="41" t="n"/>
       <c r="X977" s="41" t="n"/>
       <c r="Y977" s="41" t="n"/>
@@ -18474,6 +18496,21 @@
       <c r="AA993" s="41" t="n"/>
       <c r="AB993" s="41" t="n"/>
       <c r="AC993" s="41" t="n"/>
+    </row>
+    <row r="994">
+      <c r="E994" s="41" t="n"/>
+      <c r="F994" s="41" t="n"/>
+      <c r="G994" s="42" t="n"/>
+      <c r="J994" s="41" t="n"/>
+      <c r="K994" s="41" t="n"/>
+      <c r="L994" s="41" t="n"/>
+      <c r="W994" s="41" t="n"/>
+      <c r="X994" s="41" t="n"/>
+      <c r="Y994" s="41" t="n"/>
+      <c r="Z994" s="41" t="n"/>
+      <c r="AA994" s="41" t="n"/>
+      <c r="AB994" s="41" t="n"/>
+      <c r="AC994" s="41" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:AO48"/>

</xml_diff>